<commit_message>
Added static review using SonarLint
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18156" windowHeight="15456" tabRatio="650" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18156" windowHeight="15456" tabRatio="650" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="89">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -208,13 +208,325 @@
   </si>
   <si>
     <t>MachineId ar trebui sa fie mai mare ca 0.</t>
+  </si>
+  <si>
+    <t>Product, 99</t>
+  </si>
+  <si>
+    <t>Unnecessary Integer constructor</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">new </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>Integer(p.getPartId()).toString()</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Integer.</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>toString</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>(p.getPartId())</t>
+    </r>
+  </si>
+  <si>
+    <t>Product, 61</t>
+  </si>
+  <si>
+    <t>Remove self-assginment</t>
+  </si>
+  <si>
+    <r>
+      <t>associatedParts = associatedParts</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <t>Remove commented-out code</t>
+  </si>
+  <si>
+    <t>// = FXCollections.observableArrayList();</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Product, 11</t>
+  </si>
+  <si>
+    <t>SonarLint</t>
+  </si>
+  <si>
+    <t>Method has 8 parameters, more than 7 authorized</t>
+  </si>
+  <si>
+    <t>Changing the number of parameters at this point is a problem of which, a rather complex decision based on the architecture of the application</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">try </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(BufferedReader br = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">new </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>BufferedReader(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">new </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>FileReader(file)))</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">br = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">new </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>BufferedReader(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">new </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>FileReader(file))</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <t>InventoryService, 52</t>
+  </si>
+  <si>
+    <t>InventoryService, 60</t>
+  </si>
+  <si>
+    <t>InventoryService, 65</t>
+  </si>
+  <si>
+    <t>InventoryRepository, 28</t>
+  </si>
+  <si>
+    <t>InventoryRepository, 81</t>
+  </si>
+  <si>
+    <t>InventoryRepository, 136</t>
+  </si>
+  <si>
+    <t>Use try-with-resosurces</t>
+  </si>
+  <si>
+    <t>Sava Radu-Florian, Popa Iulian, Roszinecs Norbert</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">try </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(BufferedWriter bw = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">new </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>BufferedWriter(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">new </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>FileWriter(file)))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">bw = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">new </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>BufferedWriter(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">new </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>FileWriter(file))</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,6 +610,31 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FFA9B7C6"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FFCC7832"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FFA9B7C6"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF808080"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="5">
@@ -399,7 +736,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -434,6 +771,9 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -480,8 +820,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -796,7 +1142,7 @@
       <selection activeCell="I3" sqref="I3:J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="6"/>
     <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
@@ -808,24 +1154,24 @@
     <col min="11" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.6">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="27" t="s">
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="B2" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -834,7 +1180,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
@@ -845,14 +1191,14 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="28"/>
+      <c r="E4" s="29"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -863,14 +1209,14 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10">
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="30"/>
+      <c r="E5" s="31"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -881,26 +1227,26 @@
         <v>236</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="25"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E6" s="26"/>
+    </row>
+    <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="25"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E7" s="26"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -914,7 +1260,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="72">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -928,7 +1274,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="86.4">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -943,7 +1289,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="86.4">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
@@ -958,7 +1304,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -967,7 +1313,7 @@
       <c r="D13" s="22"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -976,7 +1322,7 @@
       <c r="D14" s="22"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -985,7 +1331,7 @@
       <c r="D15" s="22"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -994,7 +1340,7 @@
       <c r="D16" s="22"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1003,7 +1349,7 @@
       <c r="D17" s="22"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1012,7 +1358,7 @@
       <c r="D18" s="23"/>
       <c r="E18" s="15"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1021,7 +1367,7 @@
       <c r="D19" s="23"/>
       <c r="E19" s="15"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1030,7 +1376,7 @@
       <c r="D20" s="23"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1039,7 +1385,7 @@
       <c r="D21" s="23"/>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1048,7 +1394,7 @@
       <c r="D22" s="23"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1057,7 +1403,7 @@
       <c r="D23" s="23"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1066,7 +1412,7 @@
       <c r="D24" s="23"/>
       <c r="E24" s="15"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1075,7 +1421,7 @@
       <c r="D25" s="23"/>
       <c r="E25" s="15"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5">
       <c r="C27" s="11" t="s">
         <v>8</v>
       </c>
@@ -1109,7 +1455,7 @@
       <selection activeCell="J5" sqref="I3:J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="6"/>
     <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
@@ -1120,24 +1466,24 @@
     <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.6">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="27" t="s">
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="B2" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1146,7 +1492,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
@@ -1157,14 +1503,14 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="32"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -1175,14 +1521,14 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="34"/>
+      <c r="E5" s="35"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1193,26 +1539,26 @@
         <v>236</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="25"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E6" s="26"/>
+    </row>
+    <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="33">
         <v>44997</v>
       </c>
-      <c r="E7" s="25"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E7" s="26"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1226,7 +1572,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="72">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1238,7 +1584,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="43.2">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1251,7 +1597,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
@@ -1264,7 +1610,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1273,7 +1619,7 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1282,7 +1628,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1291,7 +1637,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1300,7 +1646,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1309,7 +1655,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1318,7 +1664,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1327,7 +1673,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1336,7 +1682,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1345,7 +1691,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1354,7 +1700,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1363,7 +1709,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1372,7 +1718,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1381,7 +1727,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1390,7 +1736,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5">
       <c r="C28" s="11" t="s">
         <v>8</v>
       </c>
@@ -1420,11 +1766,11 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J5" sqref="I3:J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="6"/>
     <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
@@ -1436,24 +1782,24 @@
     <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.6">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="27" t="s">
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="B2" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1462,7 +1808,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
@@ -1473,14 +1819,14 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="35"/>
+      <c r="E4" s="36"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -1491,14 +1837,14 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10">
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="37"/>
+      <c r="E5" s="38"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1509,26 +1855,26 @@
         <v>236</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="25"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E6" s="26"/>
+    </row>
+    <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="25"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E7" s="26"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1542,21 +1888,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="43.2">
       <c r="B10" s="3">
         <v>1</v>
       </c>
       <c r="C10" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="40" t="s">
+      <c r="E10" s="25" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="43.2">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1567,11 +1913,11 @@
       <c r="D11" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="40" t="s">
+      <c r="E11" s="25" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -1582,11 +1928,11 @@
       <c r="D12" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="40" t="s">
+      <c r="E12" s="25" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1594,14 +1940,14 @@
       <c r="C13" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="40" t="s">
+      <c r="D13" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="40" t="s">
+      <c r="E13" s="25" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1610,7 +1956,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1619,7 +1965,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1628,7 +1974,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1637,7 +1983,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1646,7 +1992,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1655,7 +2001,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1664,7 +2010,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1673,7 +2019,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1682,7 +2028,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1691,7 +2037,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1700,7 +2046,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1709,7 +2055,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1718,7 +2064,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1727,7 +2073,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1736,7 +2082,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1745,7 +2091,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1754,7 +2100,7 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5">
       <c r="C32" s="11" t="s">
         <v>8</v>
       </c>
@@ -1784,41 +2130,41 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="6"/>
     <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="24" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="24.109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="27.88671875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="52.5546875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="74.109375" style="6" customWidth="1"/>
     <col min="7" max="8" width="8.88671875" style="6"/>
     <col min="9" max="9" width="26.6640625" style="6" customWidth="1"/>
     <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.6">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="27" t="s">
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="B2" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1827,47 +2173,65 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I3" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="17">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="C4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
+      <c r="D4" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="36"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I4" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="3">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
+      <c r="D5" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" s="26"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I5" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="3">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
+      <c r="D6" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="26"/>
       <c r="F6" s="20"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1884,106 +2248,180 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C10" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="42" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C11" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C12" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="43.2">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C13" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="43.2">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C14" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="28.8">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C15" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C16" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" s="41" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C17" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="E17" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" s="41" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C18" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="F18" s="41" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="2"/>
+      <c r="E19" t="s">
+        <v>77</v>
+      </c>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1993,7 +2431,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2003,7 +2441,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2013,7 +2451,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2023,7 +2461,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2033,7 +2471,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2043,7 +2481,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2053,7 +2491,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2063,7 +2501,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2073,7 +2511,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2083,7 +2521,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2093,13 +2531,15 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C32" s="38" t="s">
+    <row r="32" spans="2:6">
+      <c r="C32" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="39"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="18"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="40"/>
+      <c r="F32" s="18">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>